<commit_message>
Form Register and Login
</commit_message>
<xml_diff>
--- a/Doc Vue.xlsx
+++ b/Doc Vue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Installation" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Install Bootsrap 5</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t>Install toast notification</t>
+  </si>
+  <si>
+    <t>npm i vue-toast-notification</t>
+  </si>
+  <si>
+    <t>vue-password</t>
+  </si>
+  <si>
+    <t>npm add vue-password</t>
   </si>
   <si>
     <t>Hapus template dan style di App.vue</t>
@@ -53,7 +62,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,8 +71,137 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -76,142 +214,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -222,43 +224,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -270,139 +398,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,26 +420,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -458,34 +458,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,151 +495,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -980,16 +982,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
+      <xdr:colOff>30480</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1006,7 +1008,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="617220" y="11704320"/>
+          <a:off x="586740" y="11765280"/>
           <a:ext cx="7467600" cy="1280160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1590,13 +1592,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B43:B63"/>
+  <dimension ref="B43:C74"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <sheetData>
     <row r="43" spans="2:2">
       <c r="B43" t="s">
@@ -1618,6 +1620,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="64" spans="3:3">
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1630,7 +1647,7 @@
   <sheetPr/>
   <dimension ref="B3:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
@@ -1638,22 +1655,22 @@
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1668,7 +1685,7 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fronend POST Register Done
</commit_message>
<xml_diff>
--- a/Doc Vue.xlsx
+++ b/Doc Vue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Install Bootsrap 5</t>
   </si>
@@ -31,13 +31,16 @@
     <t>Install toast notification</t>
   </si>
   <si>
-    <t>npm i vue-toast-notification</t>
-  </si>
-  <si>
     <t>vue-password</t>
   </si>
   <si>
     <t>npm add vue-password</t>
+  </si>
+  <si>
+    <t>npm i --save vue3-loading-screen</t>
+  </si>
+  <si>
+    <t>npm install epic-spinners --save</t>
   </si>
   <si>
     <t>Hapus template dan style di App.vue</t>
@@ -57,17 +60,114 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -79,85 +179,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -171,20 +194,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -193,20 +202,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +209,20 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -224,187 +233,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,8 +430,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -442,6 +451,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -457,17 +481,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,15 +516,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -518,15 +527,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -536,135 +545,136 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1592,13 +1602,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B43:C74"/>
+  <dimension ref="B43:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <sheetData>
     <row r="43" spans="2:2">
       <c r="B43" t="s">
@@ -1620,20 +1630,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="3:3">
-      <c r="C64" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="73" spans="2:2">
       <c r="B73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="2:2">
       <c r="B74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1655,22 +1673,22 @@
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
register validation submit add package pinia
</commit_message>
<xml_diff>
--- a/Doc Vue.xlsx
+++ b/Doc Vue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Install Bootsrap 5</t>
   </si>
@@ -43,6 +43,15 @@
     <t>npm install epic-spinners --save</t>
   </si>
   <si>
+    <t>npm i vee-validate --save</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> npm install -S yup   </t>
+  </si>
+  <si>
+    <t>npm install pinia</t>
+  </si>
+  <si>
     <t>Hapus template dan style di App.vue</t>
   </si>
   <si>
@@ -60,10 +69,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -88,7 +97,122 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -103,122 +227,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,187 +242,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,21 +441,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,15 +501,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -524,10 +509,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -545,40 +554,40 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -587,88 +596,88 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1602,10 +1611,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B43:B78"/>
+  <dimension ref="B43:B83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -1653,6 +1662,21 @@
     <row r="78" spans="2:2">
       <c r="B78" s="1"/>
     </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1673,22 +1697,22 @@
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
login logout with axios
</commit_message>
<xml_diff>
--- a/Doc Vue.xlsx
+++ b/Doc Vue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="23040" windowHeight="8892"/>
   </bookViews>
   <sheets>
     <sheet name="Installation" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="sidebar" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Install Bootsrap 5</t>
   </si>
@@ -50,6 +50,21 @@
   </si>
   <si>
     <t>npm install pinia</t>
+  </si>
+  <si>
+    <t>npm install vue3-cookies --save</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> npm uninstall epic-spinners</t>
+  </si>
+  <si>
+    <t>npm install vue-hooks</t>
+  </si>
+  <si>
+    <t>npm install vue-jwt-decode</t>
+  </si>
+  <si>
+    <t>npm install --save vue-axios</t>
   </si>
   <si>
     <t>Hapus template dan style di App.vue</t>
@@ -69,10 +84,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -89,6 +104,43 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -96,15 +148,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,13 +164,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -134,8 +173,60 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -143,17 +234,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -164,74 +247,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -242,187 +257,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,15 +448,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -456,6 +462,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,26 +523,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -533,18 +537,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -554,31 +569,31 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -587,97 +602,97 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1611,10 +1626,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B43:B83"/>
+  <dimension ref="B43:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="H82" sqref="H82"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -1675,6 +1690,31 @@
     <row r="83" spans="2:2">
       <c r="B83" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1697,22 +1737,22 @@
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>